<commit_message>
Coleção, variáveis, plano de testes e relatório
</commit_message>
<xml_diff>
--- a/PlanoDeTestesTrello.xlsx
+++ b/PlanoDeTestesTrello.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CURSO UDEMY\POSTMAN API AUTOMACAO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{CE712EF5-962E-483E-94B9-987204E8A670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DBA0D57-44A1-48DB-B02A-3A50D684B77C}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{CE712EF5-962E-483E-94B9-987204E8A670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD8DC7AC-F36B-4C2F-9509-B1C555B0FA45}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{DE176EE9-A5A8-4FDF-8426-19D2BABF6309}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t>TrelloAutomation</t>
   </si>
@@ -74,6 +74,53 @@
   </si>
   <si>
     <t>Enviar requisição POST assincrona para criar novo Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Content-Type is present
+- Status code: 200
+- Validating Name, Description, IdList and IdBoard
+- Response time is less than 700ms
+</t>
+  </si>
+  <si>
+    <t>Create a new card without idList.</t>
+  </si>
+  <si>
+    <t>Enviar requisição POST assincrona para criar novo Card sem o IdList</t>
+  </si>
+  <si>
+    <t>- Content-Type is present
+- Status code: 400
+- Response time is less than 300ms</t>
+  </si>
+  <si>
+    <t>Create a new card without token.</t>
+  </si>
+  <si>
+    <t>Enviar requisição POST assincrona para criar novo Card sem o token</t>
+  </si>
+  <si>
+    <t>- Content-Type is present
+- Status code: 401
+- Response time is less than 300ms</t>
+  </si>
+  <si>
+    <t>Create a new card without key.</t>
+  </si>
+  <si>
+    <t>Enviar requisição POST assincrona para criar novo Card sem a key</t>
+  </si>
+  <si>
+    <t>Update a new card.</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>/cards/{id}</t>
+  </si>
+  <si>
+    <t>Enviar requisição PUT assincrona para alterar um Card</t>
   </si>
   <si>
     <t xml:space="preserve">- Content-Type is present
@@ -81,46 +128,6 @@
 - Validating Name, Description, IdList and IdBoard
 - Response time is less than 500ms
 </t>
-  </si>
-  <si>
-    <t>Create a new card without idList.</t>
-  </si>
-  <si>
-    <t>Enviar requisição POST assincrona para criar novo Card sem o IdList</t>
-  </si>
-  <si>
-    <t>- Content-Type is present
-- Status code: 400
-- Response time is less than 300ms</t>
-  </si>
-  <si>
-    <t>Create a new card without token.</t>
-  </si>
-  <si>
-    <t>Enviar requisição POST assincrona para criar novo Card sem o token</t>
-  </si>
-  <si>
-    <t>- Content-Type is present
-- Status code: 401
-- Response time is less than 300ms</t>
-  </si>
-  <si>
-    <t>Create a new card without key.</t>
-  </si>
-  <si>
-    <t>Enviar requisição POST assincrona para criar novo Card sem a key</t>
-  </si>
-  <si>
-    <t>Update a new card.</t>
-  </si>
-  <si>
-    <t>PUT</t>
-  </si>
-  <si>
-    <t>/cards/{id}</t>
-  </si>
-  <si>
-    <t>Enviar requisição PUT assincrona para alterar um Card</t>
   </si>
   <si>
     <t>Update a card without token.</t>
@@ -674,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE37FCA-B991-418F-A1C6-DEC5E33B8D44}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -813,12 +820,12 @@
         <v>24</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45.75">
       <c r="A9" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>22</v>
@@ -830,7 +837,7 @@
         <v>23</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>18</v>
@@ -838,7 +845,7 @@
     </row>
     <row r="10" spans="1:6" ht="45.75">
       <c r="A10" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>22</v>
@@ -850,7 +857,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>18</v>
@@ -858,7 +865,7 @@
     </row>
     <row r="11" spans="1:6" ht="45.75">
       <c r="A11" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>22</v>
@@ -870,15 +877,15 @@
         <v>23</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45.75">
       <c r="A12" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>22</v>
@@ -890,7 +897,7 @@
         <v>23</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>15</v>
@@ -898,10 +905,10 @@
     </row>
     <row r="13" spans="1:6" ht="45.75">
       <c r="A13" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>9</v>
@@ -910,18 +917,18 @@
         <v>23</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45.75">
       <c r="A14" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>9</v>
@@ -930,7 +937,7 @@
         <v>23</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>18</v>
@@ -938,10 +945,10 @@
     </row>
     <row r="15" spans="1:6" ht="45.75">
       <c r="A15" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>9</v>
@@ -950,18 +957,18 @@
         <v>23</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45.75">
       <c r="A16" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>9</v>
@@ -970,7 +977,7 @@
         <v>23</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>15</v>
@@ -978,10 +985,10 @@
     </row>
     <row r="17" spans="1:6" ht="45.75">
       <c r="A17" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>9</v>
@@ -990,7 +997,7 @@
         <v>23</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>15</v>

</xml_diff>